<commit_message>
Fixed a cross-reference and dataset names
</commit_message>
<xml_diff>
--- a/datos/datos2.xlsx
+++ b/datos/datos2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bell/Library/Mobile Documents/com~apple~CloudDocs/Science/Cursos/Fund_prog/datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bell/git_repos/Bioestadistica_R/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F860D0-05D2-6F4F-8785-BC00AA2ED6CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB60B92D-02D8-4346-AE38-61C76A2D7858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,159 +35,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="310">
-  <si>
-    <t>Alpheus_lottini</t>
-  </si>
-  <si>
-    <t>Alpheus_spp</t>
-  </si>
-  <si>
-    <t>Alpheus_umbo</t>
-  </si>
-  <si>
-    <t>Amphipods</t>
-  </si>
-  <si>
-    <t>Apogon_retrosella</t>
-  </si>
-  <si>
-    <t>Appendicularians</t>
-  </si>
-  <si>
-    <t>Axoclinus_nigricaudis</t>
-  </si>
-  <si>
-    <t>Bittium_cerralvoense</t>
-  </si>
-  <si>
-    <t>Chaetognaths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cirripedia_Chthamalus_anisopoma </t>
-  </si>
-  <si>
-    <t>Cladocerans_Penila_avirostris</t>
-  </si>
-  <si>
-    <t>Cladocerans_Pseudovadne_tergestina</t>
-  </si>
-  <si>
-    <t>Copepods_Acartia_clausi</t>
-  </si>
-  <si>
-    <t>Copepods_Calanus_pacificus</t>
-  </si>
-  <si>
-    <t>Epitonium_canna</t>
-  </si>
-  <si>
-    <t>Fish_eggs</t>
-  </si>
-  <si>
-    <t>foraminifera</t>
-  </si>
-  <si>
-    <t>Gnathophyllum_panamense</t>
-  </si>
-  <si>
-    <t>Hidrozoa</t>
-  </si>
-  <si>
-    <t>Ichtyoplankton</t>
-  </si>
-  <si>
-    <t>Larvae_crustaceans_megalopa</t>
-  </si>
-  <si>
-    <t>larvae_crustaceans_zoea</t>
-  </si>
-  <si>
-    <t>Liomera_cinctimana</t>
-  </si>
-  <si>
-    <t>Litiopa_melanostoma</t>
-  </si>
-  <si>
-    <t>Mysid</t>
-  </si>
-  <si>
-    <t>Mytella_arciformis</t>
-  </si>
-  <si>
-    <t>Mytella_tumbezensis</t>
-  </si>
-  <si>
-    <t>Nanocassiope_polita</t>
-  </si>
-  <si>
-    <t>Nyctiphanes_simplex</t>
-  </si>
-  <si>
-    <t>Ostracods</t>
-  </si>
-  <si>
-    <t>Otoliths</t>
-  </si>
-  <si>
-    <t>Palaemon_ritter</t>
-  </si>
-  <si>
-    <t>Panopeus_purpureus</t>
-  </si>
-  <si>
-    <t>Parviturbo_acuticostatus</t>
-  </si>
-  <si>
-    <t>Parviturbo_erici</t>
-  </si>
-  <si>
-    <t>Parviturbo_spp</t>
-  </si>
-  <si>
-    <t>Pteropods</t>
-  </si>
-  <si>
-    <t>Quadrella_nitida</t>
-  </si>
-  <si>
-    <t>Tagelus_californianus</t>
-  </si>
-  <si>
-    <t>Tegula_globulus</t>
-  </si>
-  <si>
-    <t>Tegula_mariana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tellina_coani </t>
-  </si>
-  <si>
-    <t>Trapezia_bidentata</t>
-  </si>
-  <si>
-    <t>Trapezia_formosa</t>
-  </si>
-  <si>
-    <t>Trapezia_spp</t>
-  </si>
-  <si>
-    <t>Ulva_dactylifera</t>
-  </si>
-  <si>
-    <t>Ulva_lactuca</t>
-  </si>
-  <si>
-    <t>Ulva_spp</t>
-  </si>
-  <si>
-    <t>UOM (Unidentified Organic Material)</t>
-  </si>
-  <si>
-    <t>Datos de contenidos estomacales de especies de peces crípticos</t>
-  </si>
-  <si>
-    <t>Proyecto: Ecología trófica de peces crípticos</t>
-  </si>
   <si>
     <t>Análisis de las muestras: Marina</t>
   </si>
@@ -965,12 +812,165 @@
   <si>
     <t>Clave</t>
   </si>
+  <si>
+    <t>Proyecto: Ecología trófica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos de contenidos estomacales </t>
+  </si>
+  <si>
+    <t>Prey_1</t>
+  </si>
+  <si>
+    <t>Prey_2</t>
+  </si>
+  <si>
+    <t>Prey_3</t>
+  </si>
+  <si>
+    <t>Prey_4</t>
+  </si>
+  <si>
+    <t>Prey_5</t>
+  </si>
+  <si>
+    <t>Prey_6</t>
+  </si>
+  <si>
+    <t>Prey_7</t>
+  </si>
+  <si>
+    <t>Prey_8</t>
+  </si>
+  <si>
+    <t>Prey_9</t>
+  </si>
+  <si>
+    <t>Prey_10</t>
+  </si>
+  <si>
+    <t>Prey_11</t>
+  </si>
+  <si>
+    <t>Prey_12</t>
+  </si>
+  <si>
+    <t>Prey_13</t>
+  </si>
+  <si>
+    <t>Prey_14</t>
+  </si>
+  <si>
+    <t>Prey_15</t>
+  </si>
+  <si>
+    <t>Prey_16</t>
+  </si>
+  <si>
+    <t>Prey_17</t>
+  </si>
+  <si>
+    <t>Prey_18</t>
+  </si>
+  <si>
+    <t>Prey_19</t>
+  </si>
+  <si>
+    <t>Prey_20</t>
+  </si>
+  <si>
+    <t>Prey_21</t>
+  </si>
+  <si>
+    <t>Prey_22</t>
+  </si>
+  <si>
+    <t>Prey_23</t>
+  </si>
+  <si>
+    <t>Prey_24</t>
+  </si>
+  <si>
+    <t>Prey_25</t>
+  </si>
+  <si>
+    <t>Prey_26</t>
+  </si>
+  <si>
+    <t>Prey_27</t>
+  </si>
+  <si>
+    <t>Prey_28</t>
+  </si>
+  <si>
+    <t>Prey_29</t>
+  </si>
+  <si>
+    <t>Prey_30</t>
+  </si>
+  <si>
+    <t>Prey_31</t>
+  </si>
+  <si>
+    <t>Prey_32</t>
+  </si>
+  <si>
+    <t>Prey_33</t>
+  </si>
+  <si>
+    <t>Prey_34</t>
+  </si>
+  <si>
+    <t>Prey_35</t>
+  </si>
+  <si>
+    <t>Prey_36</t>
+  </si>
+  <si>
+    <t>Prey_37</t>
+  </si>
+  <si>
+    <t>Prey_38</t>
+  </si>
+  <si>
+    <t>Prey_39</t>
+  </si>
+  <si>
+    <t>Prey_40</t>
+  </si>
+  <si>
+    <t>Prey_41</t>
+  </si>
+  <si>
+    <t>Prey_42</t>
+  </si>
+  <si>
+    <t>Prey_43</t>
+  </si>
+  <si>
+    <t>Prey_44</t>
+  </si>
+  <si>
+    <t>Prey_45</t>
+  </si>
+  <si>
+    <t>Prey_46</t>
+  </si>
+  <si>
+    <t>Prey_47</t>
+  </si>
+  <si>
+    <t>Prey_48</t>
+  </si>
+  <si>
+    <t>Prey_49</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1101,6 +1101,12 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1807,784 +1813,784 @@
   <dimension ref="A1:IV50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:IV1"/>
+      <selection activeCell="A2" sqref="A2:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="BA1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="BB1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="BC1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
+      <c r="BD1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
+      <c r="BE1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
+      <c r="BF1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" t="s">
+      <c r="BG1" t="s">
         <v>61</v>
       </c>
-      <c r="I1" t="s">
+      <c r="BH1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" t="s">
+      <c r="BI1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" t="s">
+      <c r="BJ1" t="s">
         <v>64</v>
       </c>
-      <c r="L1" t="s">
+      <c r="BK1" t="s">
         <v>65</v>
       </c>
-      <c r="M1" t="s">
+      <c r="BL1" t="s">
         <v>66</v>
       </c>
-      <c r="N1" t="s">
+      <c r="BM1" t="s">
         <v>67</v>
       </c>
-      <c r="O1" t="s">
+      <c r="BN1" t="s">
         <v>68</v>
       </c>
-      <c r="P1" t="s">
+      <c r="BO1" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="BP1" t="s">
         <v>70</v>
       </c>
-      <c r="R1" t="s">
+      <c r="BQ1" t="s">
         <v>71</v>
       </c>
-      <c r="S1" t="s">
+      <c r="BR1" t="s">
         <v>72</v>
       </c>
-      <c r="T1" t="s">
+      <c r="BS1" t="s">
         <v>73</v>
       </c>
-      <c r="U1" t="s">
+      <c r="BT1" t="s">
         <v>74</v>
       </c>
-      <c r="V1" t="s">
+      <c r="BU1" t="s">
         <v>75</v>
       </c>
-      <c r="W1" t="s">
+      <c r="BV1" t="s">
         <v>76</v>
       </c>
-      <c r="X1" t="s">
+      <c r="BW1" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="BX1" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="BY1" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="BZ1" t="s">
         <v>80</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="CA1" t="s">
         <v>81</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="CB1" t="s">
         <v>82</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="CC1" t="s">
         <v>83</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="CD1" t="s">
         <v>84</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="CE1" t="s">
         <v>85</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="CF1" t="s">
         <v>86</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="CG1" t="s">
         <v>87</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="CH1" t="s">
         <v>88</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="CI1" t="s">
         <v>89</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="CJ1" t="s">
         <v>90</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="CK1" t="s">
         <v>91</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="CL1" t="s">
         <v>92</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="CM1" t="s">
         <v>93</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="CN1" t="s">
         <v>94</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="CO1" t="s">
         <v>95</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="CP1" t="s">
         <v>96</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="CQ1" t="s">
         <v>97</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="CR1" t="s">
         <v>98</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="CS1" t="s">
         <v>99</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="CT1" t="s">
         <v>100</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="CU1" t="s">
         <v>101</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="CV1" t="s">
         <v>102</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="CW1" t="s">
         <v>103</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="CX1" t="s">
         <v>104</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="CY1" t="s">
         <v>105</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="CZ1" t="s">
         <v>106</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="DA1" t="s">
         <v>107</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="DB1" t="s">
         <v>108</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="DC1" t="s">
         <v>109</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="DD1" t="s">
         <v>110</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="DE1" t="s">
+        <v>96</v>
+      </c>
+      <c r="DF1" t="s">
         <v>111</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="DG1" t="s">
         <v>112</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="DH1" t="s">
         <v>113</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="DI1" t="s">
         <v>114</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="DJ1" t="s">
         <v>115</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="DK1" t="s">
         <v>116</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="DL1" t="s">
         <v>117</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="DM1" t="s">
         <v>118</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="DN1" t="s">
         <v>119</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="DO1" t="s">
         <v>120</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="DP1" t="s">
         <v>121</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="DQ1" t="s">
         <v>122</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="DR1" t="s">
         <v>123</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="DS1" t="s">
         <v>124</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="DT1" t="s">
         <v>125</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="DU1" t="s">
         <v>126</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="DV1" t="s">
         <v>127</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="DW1" t="s">
         <v>128</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="DX1" t="s">
         <v>129</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="DY1" t="s">
         <v>130</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="DZ1" t="s">
         <v>131</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="EA1" t="s">
         <v>132</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="EB1" t="s">
         <v>133</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="EC1" t="s">
         <v>134</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="ED1" t="s">
         <v>135</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="EE1" t="s">
         <v>136</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="EF1" t="s">
         <v>137</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="EG1" t="s">
         <v>138</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="EH1" t="s">
         <v>139</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="EI1" t="s">
         <v>140</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="EJ1" t="s">
         <v>141</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="EK1" t="s">
         <v>142</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="EL1" t="s">
         <v>143</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="EM1" t="s">
         <v>144</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="EN1" t="s">
         <v>145</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="EO1" t="s">
         <v>146</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="EP1" t="s">
         <v>147</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="EQ1" t="s">
         <v>148</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="ER1" t="s">
         <v>149</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="ES1" t="s">
         <v>150</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="ET1" t="s">
         <v>151</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="EU1" t="s">
         <v>152</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="EV1" t="s">
         <v>153</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="EW1" t="s">
         <v>154</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="EX1" t="s">
         <v>155</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="EY1" t="s">
         <v>156</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="EZ1" t="s">
         <v>157</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="FA1" t="s">
         <v>158</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="FB1" t="s">
         <v>159</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="FC1" t="s">
         <v>160</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="FD1" t="s">
         <v>161</v>
       </c>
-      <c r="DE1" t="s">
-        <v>147</v>
-      </c>
-      <c r="DF1" t="s">
+      <c r="FE1" t="s">
         <v>162</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="FF1" t="s">
         <v>163</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="FG1" t="s">
         <v>164</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="FH1" t="s">
         <v>165</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="FI1" t="s">
         <v>166</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="FJ1" t="s">
         <v>167</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="FK1" t="s">
         <v>168</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="FL1" t="s">
         <v>169</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="FM1" t="s">
         <v>170</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="FN1" t="s">
         <v>171</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="FO1" t="s">
         <v>172</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="FP1" t="s">
         <v>173</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="FQ1" t="s">
         <v>174</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="FR1" t="s">
         <v>175</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="FS1" t="s">
         <v>176</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="FT1" t="s">
         <v>177</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="FU1" t="s">
         <v>178</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="FV1" t="s">
         <v>179</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="FW1" t="s">
         <v>180</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="FX1" t="s">
         <v>181</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="FY1" t="s">
         <v>182</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="FZ1" t="s">
         <v>183</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="GA1" t="s">
         <v>184</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="GB1" t="s">
         <v>185</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="GC1" t="s">
         <v>186</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="GD1" t="s">
         <v>187</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="GE1" t="s">
         <v>188</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="GF1" t="s">
         <v>189</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="GG1" t="s">
         <v>190</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="GH1" t="s">
         <v>191</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="GI1" t="s">
         <v>192</v>
       </c>
-      <c r="EK1" t="s">
+      <c r="GJ1" t="s">
         <v>193</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="GK1" t="s">
         <v>194</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="GL1" t="s">
         <v>195</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="GM1" t="s">
         <v>196</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="GN1" t="s">
         <v>197</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="GO1" t="s">
         <v>198</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="GP1" t="s">
         <v>199</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="GQ1" t="s">
         <v>200</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="GR1" t="s">
         <v>201</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="GS1" t="s">
         <v>202</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="GT1" t="s">
         <v>203</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="GU1" t="s">
         <v>204</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="GV1" t="s">
         <v>205</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="GW1" t="s">
         <v>206</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="GX1" t="s">
         <v>207</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="GY1" t="s">
         <v>208</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="GZ1" t="s">
         <v>209</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="HA1" t="s">
         <v>210</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="HB1" t="s">
         <v>211</v>
       </c>
-      <c r="FD1" t="s">
+      <c r="HC1" t="s">
         <v>212</v>
       </c>
-      <c r="FE1" t="s">
+      <c r="HD1" t="s">
         <v>213</v>
       </c>
-      <c r="FF1" t="s">
+      <c r="HE1" t="s">
         <v>214</v>
       </c>
-      <c r="FG1" t="s">
+      <c r="HF1" t="s">
         <v>215</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="HG1" t="s">
         <v>216</v>
       </c>
-      <c r="FI1" t="s">
+      <c r="HH1" t="s">
         <v>217</v>
       </c>
-      <c r="FJ1" t="s">
+      <c r="HI1" t="s">
         <v>218</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="HJ1" t="s">
         <v>219</v>
       </c>
-      <c r="FL1" t="s">
+      <c r="HK1" t="s">
         <v>220</v>
       </c>
-      <c r="FM1" t="s">
+      <c r="HL1" t="s">
         <v>221</v>
       </c>
-      <c r="FN1" t="s">
+      <c r="HM1" t="s">
         <v>222</v>
       </c>
-      <c r="FO1" t="s">
+      <c r="HN1" t="s">
         <v>223</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="HO1" t="s">
         <v>224</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="HP1" t="s">
         <v>225</v>
       </c>
-      <c r="FR1" t="s">
+      <c r="HQ1" t="s">
         <v>226</v>
       </c>
-      <c r="FS1" t="s">
+      <c r="HR1" t="s">
         <v>227</v>
       </c>
-      <c r="FT1" t="s">
+      <c r="HS1" t="s">
         <v>228</v>
       </c>
-      <c r="FU1" t="s">
+      <c r="HT1" t="s">
         <v>229</v>
       </c>
-      <c r="FV1" t="s">
+      <c r="HU1" t="s">
         <v>230</v>
       </c>
-      <c r="FW1" t="s">
+      <c r="HV1" t="s">
         <v>231</v>
       </c>
-      <c r="FX1" t="s">
+      <c r="HW1" t="s">
         <v>232</v>
       </c>
-      <c r="FY1" t="s">
+      <c r="HX1" t="s">
         <v>233</v>
       </c>
-      <c r="FZ1" t="s">
+      <c r="HY1" t="s">
         <v>234</v>
       </c>
-      <c r="GA1" t="s">
+      <c r="HZ1" t="s">
         <v>235</v>
       </c>
-      <c r="GB1" t="s">
+      <c r="IA1" t="s">
         <v>236</v>
       </c>
-      <c r="GC1" t="s">
+      <c r="IB1" t="s">
         <v>237</v>
       </c>
-      <c r="GD1" t="s">
+      <c r="IC1" t="s">
         <v>238</v>
       </c>
-      <c r="GE1" t="s">
+      <c r="ID1" t="s">
         <v>239</v>
       </c>
-      <c r="GF1" t="s">
+      <c r="IE1" t="s">
         <v>240</v>
       </c>
-      <c r="GG1" t="s">
+      <c r="IF1" t="s">
         <v>241</v>
       </c>
-      <c r="GH1" t="s">
+      <c r="IG1" t="s">
         <v>242</v>
       </c>
-      <c r="GI1" t="s">
+      <c r="IH1" t="s">
         <v>243</v>
       </c>
-      <c r="GJ1" t="s">
+      <c r="II1" t="s">
         <v>244</v>
       </c>
-      <c r="GK1" t="s">
+      <c r="IJ1" t="s">
         <v>245</v>
       </c>
-      <c r="GL1" t="s">
+      <c r="IK1" t="s">
         <v>246</v>
       </c>
-      <c r="GM1" t="s">
+      <c r="IL1" t="s">
         <v>247</v>
       </c>
-      <c r="GN1" t="s">
+      <c r="IM1" t="s">
         <v>248</v>
       </c>
-      <c r="GO1" t="s">
+      <c r="IN1" t="s">
         <v>249</v>
       </c>
-      <c r="GP1" t="s">
+      <c r="IO1" t="s">
         <v>250</v>
       </c>
-      <c r="GQ1" t="s">
+      <c r="IP1" t="s">
         <v>251</v>
       </c>
-      <c r="GR1" t="s">
+      <c r="IQ1" t="s">
         <v>252</v>
       </c>
-      <c r="GS1" t="s">
+      <c r="IR1" t="s">
         <v>253</v>
       </c>
-      <c r="GT1" t="s">
+      <c r="IS1" t="s">
         <v>254</v>
       </c>
-      <c r="GU1" t="s">
+      <c r="IT1" t="s">
         <v>255</v>
       </c>
-      <c r="GV1" t="s">
+      <c r="IU1" t="s">
         <v>256</v>
       </c>
-      <c r="GW1" t="s">
+      <c r="IV1" t="s">
         <v>257</v>
-      </c>
-      <c r="GX1" t="s">
-        <v>258</v>
-      </c>
-      <c r="GY1" t="s">
-        <v>259</v>
-      </c>
-      <c r="GZ1" t="s">
-        <v>260</v>
-      </c>
-      <c r="HA1" t="s">
-        <v>261</v>
-      </c>
-      <c r="HB1" t="s">
-        <v>262</v>
-      </c>
-      <c r="HC1" t="s">
-        <v>263</v>
-      </c>
-      <c r="HD1" t="s">
-        <v>264</v>
-      </c>
-      <c r="HE1" t="s">
-        <v>265</v>
-      </c>
-      <c r="HF1" t="s">
-        <v>266</v>
-      </c>
-      <c r="HG1" t="s">
-        <v>267</v>
-      </c>
-      <c r="HH1" t="s">
-        <v>268</v>
-      </c>
-      <c r="HI1" t="s">
-        <v>269</v>
-      </c>
-      <c r="HJ1" t="s">
-        <v>270</v>
-      </c>
-      <c r="HK1" t="s">
-        <v>271</v>
-      </c>
-      <c r="HL1" t="s">
-        <v>272</v>
-      </c>
-      <c r="HM1" t="s">
-        <v>273</v>
-      </c>
-      <c r="HN1" t="s">
-        <v>274</v>
-      </c>
-      <c r="HO1" t="s">
-        <v>275</v>
-      </c>
-      <c r="HP1" t="s">
-        <v>276</v>
-      </c>
-      <c r="HQ1" t="s">
-        <v>277</v>
-      </c>
-      <c r="HR1" t="s">
-        <v>278</v>
-      </c>
-      <c r="HS1" t="s">
-        <v>279</v>
-      </c>
-      <c r="HT1" t="s">
-        <v>280</v>
-      </c>
-      <c r="HU1" t="s">
-        <v>281</v>
-      </c>
-      <c r="HV1" t="s">
-        <v>282</v>
-      </c>
-      <c r="HW1" t="s">
-        <v>283</v>
-      </c>
-      <c r="HX1" t="s">
-        <v>284</v>
-      </c>
-      <c r="HY1" t="s">
-        <v>285</v>
-      </c>
-      <c r="HZ1" t="s">
-        <v>286</v>
-      </c>
-      <c r="IA1" t="s">
-        <v>287</v>
-      </c>
-      <c r="IB1" t="s">
-        <v>288</v>
-      </c>
-      <c r="IC1" t="s">
-        <v>289</v>
-      </c>
-      <c r="ID1" t="s">
-        <v>290</v>
-      </c>
-      <c r="IE1" t="s">
-        <v>291</v>
-      </c>
-      <c r="IF1" t="s">
-        <v>292</v>
-      </c>
-      <c r="IG1" t="s">
-        <v>293</v>
-      </c>
-      <c r="IH1" t="s">
-        <v>294</v>
-      </c>
-      <c r="II1" t="s">
-        <v>295</v>
-      </c>
-      <c r="IJ1" t="s">
-        <v>296</v>
-      </c>
-      <c r="IK1" t="s">
-        <v>297</v>
-      </c>
-      <c r="IL1" t="s">
-        <v>298</v>
-      </c>
-      <c r="IM1" t="s">
-        <v>299</v>
-      </c>
-      <c r="IN1" t="s">
-        <v>300</v>
-      </c>
-      <c r="IO1" t="s">
-        <v>301</v>
-      </c>
-      <c r="IP1" t="s">
-        <v>302</v>
-      </c>
-      <c r="IQ1" t="s">
-        <v>303</v>
-      </c>
-      <c r="IR1" t="s">
-        <v>304</v>
-      </c>
-      <c r="IS1" t="s">
-        <v>305</v>
-      </c>
-      <c r="IT1" t="s">
-        <v>306</v>
-      </c>
-      <c r="IU1" t="s">
-        <v>307</v>
-      </c>
-      <c r="IV1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>261</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3354,7 +3360,7 @@
     </row>
     <row r="3" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>262</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4124,7 +4130,7 @@
     </row>
     <row r="4" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>263</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4894,7 +4900,7 @@
     </row>
     <row r="5" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>264</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -5664,7 +5670,7 @@
     </row>
     <row r="6" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>265</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -6434,7 +6440,7 @@
     </row>
     <row r="7" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>266</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -7204,7 +7210,7 @@
     </row>
     <row r="8" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>267</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -7974,7 +7980,7 @@
     </row>
     <row r="9" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>268</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -8744,7 +8750,7 @@
     </row>
     <row r="10" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>269</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -9514,7 +9520,7 @@
     </row>
     <row r="11" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>270</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -10284,7 +10290,7 @@
     </row>
     <row r="12" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>271</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -11054,7 +11060,7 @@
     </row>
     <row r="13" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>272</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -11824,7 +11830,7 @@
     </row>
     <row r="14" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>273</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -12594,7 +12600,7 @@
     </row>
     <row r="15" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>274</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -13364,7 +13370,7 @@
     </row>
     <row r="16" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>275</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -14134,7 +14140,7 @@
     </row>
     <row r="17" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -14904,7 +14910,7 @@
     </row>
     <row r="18" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>277</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -15674,7 +15680,7 @@
     </row>
     <row r="19" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>278</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -16444,7 +16450,7 @@
     </row>
     <row r="20" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>279</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -17214,7 +17220,7 @@
     </row>
     <row r="21" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>280</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -17984,7 +17990,7 @@
     </row>
     <row r="22" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>281</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -18754,7 +18760,7 @@
     </row>
     <row r="23" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>282</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -19524,7 +19530,7 @@
     </row>
     <row r="24" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>283</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -20294,7 +20300,7 @@
     </row>
     <row r="25" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>284</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -21064,7 +21070,7 @@
     </row>
     <row r="26" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>285</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -21834,7 +21840,7 @@
     </row>
     <row r="27" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>286</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -22604,7 +22610,7 @@
     </row>
     <row r="28" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>287</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -23374,7 +23380,7 @@
     </row>
     <row r="29" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>288</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -24144,7 +24150,7 @@
     </row>
     <row r="30" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>289</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -24914,7 +24920,7 @@
     </row>
     <row r="31" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>290</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -25684,7 +25690,7 @@
     </row>
     <row r="32" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>291</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -26454,7 +26460,7 @@
     </row>
     <row r="33" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>292</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -27224,7 +27230,7 @@
     </row>
     <row r="34" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>293</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -27994,7 +28000,7 @@
     </row>
     <row r="35" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>294</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -28764,7 +28770,7 @@
     </row>
     <row r="36" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>295</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -29534,7 +29540,7 @@
     </row>
     <row r="37" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>296</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -30304,7 +30310,7 @@
     </row>
     <row r="38" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>297</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -31074,7 +31080,7 @@
     </row>
     <row r="39" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>298</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -31844,7 +31850,7 @@
     </row>
     <row r="40" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>299</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -32614,7 +32620,7 @@
     </row>
     <row r="41" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>300</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -33384,7 +33390,7 @@
     </row>
     <row r="42" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>301</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -34154,7 +34160,7 @@
     </row>
     <row r="43" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>302</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -34924,7 +34930,7 @@
     </row>
     <row r="44" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>303</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -35694,7 +35700,7 @@
     </row>
     <row r="45" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>304</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -36464,7 +36470,7 @@
     </row>
     <row r="46" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>305</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -37234,7 +37240,7 @@
     </row>
     <row r="47" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>306</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -38004,7 +38010,7 @@
     </row>
     <row r="48" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>307</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -38774,7 +38780,7 @@
     </row>
     <row r="49" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>308</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -39544,7 +39550,7 @@
     </row>
     <row r="50" spans="1:256" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>309</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -40313,6 +40319,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -40322,191 +40329,191 @@
   <dimension ref="A1:AX261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="B6" sqref="B6:AX6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" t="s">
+        <v>266</v>
+      </c>
+      <c r="H6" t="s">
+        <v>267</v>
+      </c>
+      <c r="I6" t="s">
+        <v>268</v>
+      </c>
+      <c r="J6" t="s">
+        <v>269</v>
+      </c>
+      <c r="K6" t="s">
+        <v>270</v>
+      </c>
+      <c r="L6" t="s">
+        <v>271</v>
+      </c>
+      <c r="M6" t="s">
+        <v>272</v>
+      </c>
+      <c r="N6" t="s">
+        <v>273</v>
+      </c>
+      <c r="O6" t="s">
+        <v>274</v>
+      </c>
+      <c r="P6" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>276</v>
+      </c>
+      <c r="R6" t="s">
+        <v>277</v>
+      </c>
+      <c r="S6" t="s">
+        <v>278</v>
+      </c>
+      <c r="T6" t="s">
+        <v>279</v>
+      </c>
+      <c r="U6" t="s">
+        <v>280</v>
+      </c>
+      <c r="V6" t="s">
+        <v>281</v>
+      </c>
+      <c r="W6" t="s">
+        <v>282</v>
+      </c>
+      <c r="X6" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>284</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>286</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>287</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>288</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>289</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>290</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>291</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>292</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>293</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>294</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>295</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>296</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>297</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>298</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>299</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>300</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>301</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>302</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>303</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>304</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>305</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>306</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>307</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>308</v>
+      </c>
+      <c r="AX6" t="s">
         <v>309</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S6" t="s">
-        <v>17</v>
-      </c>
-      <c r="T6" t="s">
-        <v>18</v>
-      </c>
-      <c r="U6" t="s">
-        <v>19</v>
-      </c>
-      <c r="V6" t="s">
-        <v>20</v>
-      </c>
-      <c r="W6" t="s">
-        <v>21</v>
-      </c>
-      <c r="X6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -40658,7 +40665,7 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -40810,7 +40817,7 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -40962,7 +40969,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -41114,7 +41121,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -41266,7 +41273,7 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -41418,7 +41425,7 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -41570,7 +41577,7 @@
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -41722,7 +41729,7 @@
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -41874,7 +41881,7 @@
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -42026,7 +42033,7 @@
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -42178,7 +42185,7 @@
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -42330,7 +42337,7 @@
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -42482,7 +42489,7 @@
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -42634,7 +42641,7 @@
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -42786,7 +42793,7 @@
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -42938,7 +42945,7 @@
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -43090,7 +43097,7 @@
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -43242,7 +43249,7 @@
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -43394,7 +43401,7 @@
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -43546,7 +43553,7 @@
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -43698,7 +43705,7 @@
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -43850,7 +43857,7 @@
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -44002,7 +44009,7 @@
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -44154,7 +44161,7 @@
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -44306,7 +44313,7 @@
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -44458,7 +44465,7 @@
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -44610,7 +44617,7 @@
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -44762,7 +44769,7 @@
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -44914,7 +44921,7 @@
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -45066,7 +45073,7 @@
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -45218,7 +45225,7 @@
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -45370,7 +45377,7 @@
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -45522,7 +45529,7 @@
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -45674,7 +45681,7 @@
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -45826,7 +45833,7 @@
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -45978,7 +45985,7 @@
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -46130,7 +46137,7 @@
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -46282,7 +46289,7 @@
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -46434,7 +46441,7 @@
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -46586,7 +46593,7 @@
     </row>
     <row r="47" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -46738,7 +46745,7 @@
     </row>
     <row r="48" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -46890,7 +46897,7 @@
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -47042,7 +47049,7 @@
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -47194,7 +47201,7 @@
     </row>
     <row r="51" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -47346,7 +47353,7 @@
     </row>
     <row r="52" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -47498,7 +47505,7 @@
     </row>
     <row r="53" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -47650,7 +47657,7 @@
     </row>
     <row r="54" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -47802,7 +47809,7 @@
     </row>
     <row r="55" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -47954,7 +47961,7 @@
     </row>
     <row r="56" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -48106,7 +48113,7 @@
     </row>
     <row r="57" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -48258,7 +48265,7 @@
     </row>
     <row r="58" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -48410,7 +48417,7 @@
     </row>
     <row r="59" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -48562,7 +48569,7 @@
     </row>
     <row r="60" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -48714,7 +48721,7 @@
     </row>
     <row r="61" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -48866,7 +48873,7 @@
     </row>
     <row r="62" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -49018,7 +49025,7 @@
     </row>
     <row r="63" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -49170,7 +49177,7 @@
     </row>
     <row r="64" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -49322,7 +49329,7 @@
     </row>
     <row r="65" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -49474,7 +49481,7 @@
     </row>
     <row r="66" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -49626,7 +49633,7 @@
     </row>
     <row r="67" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -49778,7 +49785,7 @@
     </row>
     <row r="68" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -49930,7 +49937,7 @@
     </row>
     <row r="69" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -50082,7 +50089,7 @@
     </row>
     <row r="70" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -50234,7 +50241,7 @@
     </row>
     <row r="71" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -50386,7 +50393,7 @@
     </row>
     <row r="72" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -50538,7 +50545,7 @@
     </row>
     <row r="73" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -50690,7 +50697,7 @@
     </row>
     <row r="74" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -50842,7 +50849,7 @@
     </row>
     <row r="75" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -50994,7 +51001,7 @@
     </row>
     <row r="76" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -51146,7 +51153,7 @@
     </row>
     <row r="77" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -51298,7 +51305,7 @@
     </row>
     <row r="78" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -51450,7 +51457,7 @@
     </row>
     <row r="79" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -51602,7 +51609,7 @@
     </row>
     <row r="80" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -51754,7 +51761,7 @@
     </row>
     <row r="81" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -51906,7 +51913,7 @@
     </row>
     <row r="82" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -52058,7 +52065,7 @@
     </row>
     <row r="83" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -52210,7 +52217,7 @@
     </row>
     <row r="84" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -52362,7 +52369,7 @@
     </row>
     <row r="85" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -52514,7 +52521,7 @@
     </row>
     <row r="86" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -52666,7 +52673,7 @@
     </row>
     <row r="87" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -52818,7 +52825,7 @@
     </row>
     <row r="88" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -52970,7 +52977,7 @@
     </row>
     <row r="89" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -53122,7 +53129,7 @@
     </row>
     <row r="90" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -53274,7 +53281,7 @@
     </row>
     <row r="91" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -53426,7 +53433,7 @@
     </row>
     <row r="92" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -53578,7 +53585,7 @@
     </row>
     <row r="93" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -53730,7 +53737,7 @@
     </row>
     <row r="94" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -53882,7 +53889,7 @@
     </row>
     <row r="95" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -54034,7 +54041,7 @@
     </row>
     <row r="96" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -54186,7 +54193,7 @@
     </row>
     <row r="97" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -54338,7 +54345,7 @@
     </row>
     <row r="98" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -54490,7 +54497,7 @@
     </row>
     <row r="99" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -54642,7 +54649,7 @@
     </row>
     <row r="100" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -54794,7 +54801,7 @@
     </row>
     <row r="101" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -54946,7 +54953,7 @@
     </row>
     <row r="102" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -55098,7 +55105,7 @@
     </row>
     <row r="103" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -55250,7 +55257,7 @@
     </row>
     <row r="104" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -55402,7 +55409,7 @@
     </row>
     <row r="105" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -55554,7 +55561,7 @@
     </row>
     <row r="106" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -55706,7 +55713,7 @@
     </row>
     <row r="107" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -55858,7 +55865,7 @@
     </row>
     <row r="108" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>156</v>
+        <v>105</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -56010,7 +56017,7 @@
     </row>
     <row r="109" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -56162,7 +56169,7 @@
     </row>
     <row r="110" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>158</v>
+        <v>107</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -56314,7 +56321,7 @@
     </row>
     <row r="111" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>159</v>
+        <v>108</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -56466,7 +56473,7 @@
     </row>
     <row r="112" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>160</v>
+        <v>109</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -56618,7 +56625,7 @@
     </row>
     <row r="113" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -56770,7 +56777,7 @@
     </row>
     <row r="114" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -56922,7 +56929,7 @@
     </row>
     <row r="115" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -57074,7 +57081,7 @@
     </row>
     <row r="116" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>163</v>
+        <v>112</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -57226,7 +57233,7 @@
     </row>
     <row r="117" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>164</v>
+        <v>113</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -57378,7 +57385,7 @@
     </row>
     <row r="118" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -57530,7 +57537,7 @@
     </row>
     <row r="119" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -57682,7 +57689,7 @@
     </row>
     <row r="120" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -57834,7 +57841,7 @@
     </row>
     <row r="121" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -57986,7 +57993,7 @@
     </row>
     <row r="122" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -58138,7 +58145,7 @@
     </row>
     <row r="123" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>170</v>
+        <v>119</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -58290,7 +58297,7 @@
     </row>
     <row r="124" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>171</v>
+        <v>120</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -58442,7 +58449,7 @@
     </row>
     <row r="125" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>172</v>
+        <v>121</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -58594,7 +58601,7 @@
     </row>
     <row r="126" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>173</v>
+        <v>122</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -58746,7 +58753,7 @@
     </row>
     <row r="127" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -58898,7 +58905,7 @@
     </row>
     <row r="128" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -59050,7 +59057,7 @@
     </row>
     <row r="129" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -59202,7 +59209,7 @@
     </row>
     <row r="130" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -59354,7 +59361,7 @@
     </row>
     <row r="131" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -59506,7 +59513,7 @@
     </row>
     <row r="132" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -59658,7 +59665,7 @@
     </row>
     <row r="133" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -59810,7 +59817,7 @@
     </row>
     <row r="134" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -59962,7 +59969,7 @@
     </row>
     <row r="135" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>182</v>
+        <v>131</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -60114,7 +60121,7 @@
     </row>
     <row r="136" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>183</v>
+        <v>132</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -60266,7 +60273,7 @@
     </row>
     <row r="137" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -60418,7 +60425,7 @@
     </row>
     <row r="138" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>185</v>
+        <v>134</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -60570,7 +60577,7 @@
     </row>
     <row r="139" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -60722,7 +60729,7 @@
     </row>
     <row r="140" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -60874,7 +60881,7 @@
     </row>
     <row r="141" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -61026,7 +61033,7 @@
     </row>
     <row r="142" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>189</v>
+        <v>138</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -61178,7 +61185,7 @@
     </row>
     <row r="143" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>190</v>
+        <v>139</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -61330,7 +61337,7 @@
     </row>
     <row r="144" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -61482,7 +61489,7 @@
     </row>
     <row r="145" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>192</v>
+        <v>141</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -61634,7 +61641,7 @@
     </row>
     <row r="146" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>193</v>
+        <v>142</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -61786,7 +61793,7 @@
     </row>
     <row r="147" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -61938,7 +61945,7 @@
     </row>
     <row r="148" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>195</v>
+        <v>144</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -62090,7 +62097,7 @@
     </row>
     <row r="149" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -62242,7 +62249,7 @@
     </row>
     <row r="150" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -62394,7 +62401,7 @@
     </row>
     <row r="151" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -62546,7 +62553,7 @@
     </row>
     <row r="152" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>199</v>
+        <v>148</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -62698,7 +62705,7 @@
     </row>
     <row r="153" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -62850,7 +62857,7 @@
     </row>
     <row r="154" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -63002,7 +63009,7 @@
     </row>
     <row r="155" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>202</v>
+        <v>151</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -63154,7 +63161,7 @@
     </row>
     <row r="156" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -63306,7 +63313,7 @@
     </row>
     <row r="157" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -63458,7 +63465,7 @@
     </row>
     <row r="158" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -63610,7 +63617,7 @@
     </row>
     <row r="159" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>206</v>
+        <v>155</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -63762,7 +63769,7 @@
     </row>
     <row r="160" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>207</v>
+        <v>156</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -63914,7 +63921,7 @@
     </row>
     <row r="161" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>208</v>
+        <v>157</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -64066,7 +64073,7 @@
     </row>
     <row r="162" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>209</v>
+        <v>158</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -64218,7 +64225,7 @@
     </row>
     <row r="163" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>210</v>
+        <v>159</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -64370,7 +64377,7 @@
     </row>
     <row r="164" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>211</v>
+        <v>160</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -64522,7 +64529,7 @@
     </row>
     <row r="165" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -64674,7 +64681,7 @@
     </row>
     <row r="166" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>213</v>
+        <v>162</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -64826,7 +64833,7 @@
     </row>
     <row r="167" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>214</v>
+        <v>163</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -64978,7 +64985,7 @@
     </row>
     <row r="168" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>215</v>
+        <v>164</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -65130,7 +65137,7 @@
     </row>
     <row r="169" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>216</v>
+        <v>165</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -65282,7 +65289,7 @@
     </row>
     <row r="170" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -65434,7 +65441,7 @@
     </row>
     <row r="171" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>218</v>
+        <v>167</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -65586,7 +65593,7 @@
     </row>
     <row r="172" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>219</v>
+        <v>168</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -65738,7 +65745,7 @@
     </row>
     <row r="173" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>220</v>
+        <v>169</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -65890,7 +65897,7 @@
     </row>
     <row r="174" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>221</v>
+        <v>170</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -66042,7 +66049,7 @@
     </row>
     <row r="175" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>222</v>
+        <v>171</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -66194,7 +66201,7 @@
     </row>
     <row r="176" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>223</v>
+        <v>172</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -66346,7 +66353,7 @@
     </row>
     <row r="177" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -66498,7 +66505,7 @@
     </row>
     <row r="178" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>225</v>
+        <v>174</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -66650,7 +66657,7 @@
     </row>
     <row r="179" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>226</v>
+        <v>175</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -66802,7 +66809,7 @@
     </row>
     <row r="180" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -66954,7 +66961,7 @@
     </row>
     <row r="181" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -67106,7 +67113,7 @@
     </row>
     <row r="182" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>229</v>
+        <v>178</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -67258,7 +67265,7 @@
     </row>
     <row r="183" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>230</v>
+        <v>179</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -67410,7 +67417,7 @@
     </row>
     <row r="184" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -67562,7 +67569,7 @@
     </row>
     <row r="185" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>232</v>
+        <v>181</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -67714,7 +67721,7 @@
     </row>
     <row r="186" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>233</v>
+        <v>182</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -67866,7 +67873,7 @@
     </row>
     <row r="187" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -68018,7 +68025,7 @@
     </row>
     <row r="188" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>235</v>
+        <v>184</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -68170,7 +68177,7 @@
     </row>
     <row r="189" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>236</v>
+        <v>185</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -68322,7 +68329,7 @@
     </row>
     <row r="190" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -68474,7 +68481,7 @@
     </row>
     <row r="191" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>238</v>
+        <v>187</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -68626,7 +68633,7 @@
     </row>
     <row r="192" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -68778,7 +68785,7 @@
     </row>
     <row r="193" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -68930,7 +68937,7 @@
     </row>
     <row r="194" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>241</v>
+        <v>190</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -69082,7 +69089,7 @@
     </row>
     <row r="195" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>242</v>
+        <v>191</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -69234,7 +69241,7 @@
     </row>
     <row r="196" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>243</v>
+        <v>192</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -69386,7 +69393,7 @@
     </row>
     <row r="197" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -69538,7 +69545,7 @@
     </row>
     <row r="198" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -69690,7 +69697,7 @@
     </row>
     <row r="199" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -69842,7 +69849,7 @@
     </row>
     <row r="200" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -69994,7 +70001,7 @@
     </row>
     <row r="201" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -70146,7 +70153,7 @@
     </row>
     <row r="202" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -70298,7 +70305,7 @@
     </row>
     <row r="203" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>250</v>
+        <v>199</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -70450,7 +70457,7 @@
     </row>
     <row r="204" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>251</v>
+        <v>200</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -70602,7 +70609,7 @@
     </row>
     <row r="205" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>252</v>
+        <v>201</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -70754,7 +70761,7 @@
     </row>
     <row r="206" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>253</v>
+        <v>202</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -70906,7 +70913,7 @@
     </row>
     <row r="207" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -71058,7 +71065,7 @@
     </row>
     <row r="208" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -71210,7 +71217,7 @@
     </row>
     <row r="209" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>256</v>
+        <v>205</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -71362,7 +71369,7 @@
     </row>
     <row r="210" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>257</v>
+        <v>206</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -71514,7 +71521,7 @@
     </row>
     <row r="211" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>258</v>
+        <v>207</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -71666,7 +71673,7 @@
     </row>
     <row r="212" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>259</v>
+        <v>208</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -71818,7 +71825,7 @@
     </row>
     <row r="213" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>260</v>
+        <v>209</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -71970,7 +71977,7 @@
     </row>
     <row r="214" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -72122,7 +72129,7 @@
     </row>
     <row r="215" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>262</v>
+        <v>211</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -72274,7 +72281,7 @@
     </row>
     <row r="216" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>263</v>
+        <v>212</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -72426,7 +72433,7 @@
     </row>
     <row r="217" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>264</v>
+        <v>213</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -72578,7 +72585,7 @@
     </row>
     <row r="218" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>265</v>
+        <v>214</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -72730,7 +72737,7 @@
     </row>
     <row r="219" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>266</v>
+        <v>215</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -72882,7 +72889,7 @@
     </row>
     <row r="220" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>267</v>
+        <v>216</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -73034,7 +73041,7 @@
     </row>
     <row r="221" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>268</v>
+        <v>217</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -73186,7 +73193,7 @@
     </row>
     <row r="222" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>269</v>
+        <v>218</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -73338,7 +73345,7 @@
     </row>
     <row r="223" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>270</v>
+        <v>219</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -73490,7 +73497,7 @@
     </row>
     <row r="224" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>271</v>
+        <v>220</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -73642,7 +73649,7 @@
     </row>
     <row r="225" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>272</v>
+        <v>221</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -73794,7 +73801,7 @@
     </row>
     <row r="226" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>273</v>
+        <v>222</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -73946,7 +73953,7 @@
     </row>
     <row r="227" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>274</v>
+        <v>223</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -74098,7 +74105,7 @@
     </row>
     <row r="228" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>275</v>
+        <v>224</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -74250,7 +74257,7 @@
     </row>
     <row r="229" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -74402,7 +74409,7 @@
     </row>
     <row r="230" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>277</v>
+        <v>226</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -74554,7 +74561,7 @@
     </row>
     <row r="231" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>278</v>
+        <v>227</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -74706,7 +74713,7 @@
     </row>
     <row r="232" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>279</v>
+        <v>228</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -74858,7 +74865,7 @@
     </row>
     <row r="233" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>280</v>
+        <v>229</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -75010,7 +75017,7 @@
     </row>
     <row r="234" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>281</v>
+        <v>230</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -75162,7 +75169,7 @@
     </row>
     <row r="235" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>282</v>
+        <v>231</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -75314,7 +75321,7 @@
     </row>
     <row r="236" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>283</v>
+        <v>232</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -75466,7 +75473,7 @@
     </row>
     <row r="237" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>284</v>
+        <v>233</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -75618,7 +75625,7 @@
     </row>
     <row r="238" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>285</v>
+        <v>234</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -75770,7 +75777,7 @@
     </row>
     <row r="239" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>286</v>
+        <v>235</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -75922,7 +75929,7 @@
     </row>
     <row r="240" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>287</v>
+        <v>236</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -76074,7 +76081,7 @@
     </row>
     <row r="241" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="B241">
         <v>0</v>
@@ -76226,7 +76233,7 @@
     </row>
     <row r="242" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -76378,7 +76385,7 @@
     </row>
     <row r="243" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>290</v>
+        <v>239</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -76530,7 +76537,7 @@
     </row>
     <row r="244" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>291</v>
+        <v>240</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -76682,7 +76689,7 @@
     </row>
     <row r="245" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>292</v>
+        <v>241</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -76834,7 +76841,7 @@
     </row>
     <row r="246" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>293</v>
+        <v>242</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -76986,7 +76993,7 @@
     </row>
     <row r="247" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>294</v>
+        <v>243</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -77138,7 +77145,7 @@
     </row>
     <row r="248" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>295</v>
+        <v>244</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -77290,7 +77297,7 @@
     </row>
     <row r="249" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>296</v>
+        <v>245</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -77442,7 +77449,7 @@
     </row>
     <row r="250" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>297</v>
+        <v>246</v>
       </c>
       <c r="B250">
         <v>0</v>
@@ -77594,7 +77601,7 @@
     </row>
     <row r="251" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>298</v>
+        <v>247</v>
       </c>
       <c r="B251">
         <v>0</v>
@@ -77746,7 +77753,7 @@
     </row>
     <row r="252" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="B252">
         <v>0</v>
@@ -77898,7 +77905,7 @@
     </row>
     <row r="253" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="B253">
         <v>0</v>
@@ -78050,7 +78057,7 @@
     </row>
     <row r="254" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>301</v>
+        <v>250</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -78202,7 +78209,7 @@
     </row>
     <row r="255" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="B255">
         <v>0</v>
@@ -78354,7 +78361,7 @@
     </row>
     <row r="256" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>303</v>
+        <v>252</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -78506,7 +78513,7 @@
     </row>
     <row r="257" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>304</v>
+        <v>253</v>
       </c>
       <c r="B257">
         <v>0</v>
@@ -78658,7 +78665,7 @@
     </row>
     <row r="258" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>305</v>
+        <v>254</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -78810,7 +78817,7 @@
     </row>
     <row r="259" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>306</v>
+        <v>255</v>
       </c>
       <c r="B259">
         <v>0</v>
@@ -78962,7 +78969,7 @@
     </row>
     <row r="260" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>307</v>
+        <v>256</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -79114,7 +79121,7 @@
     </row>
     <row r="261" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>308</v>
+        <v>257</v>
       </c>
       <c r="B261">
         <v>0</v>

</xml_diff>